<commit_message>
Updated data source features
</commit_message>
<xml_diff>
--- a/financial_models/Model_templates/Listed_template/Stock_Valuation.xlsx
+++ b/financial_models/Model_templates/Listed_template/Stock_Valuation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry.chen\PycharmProjects\Invest_Proc\financial_models\Model_templates\Listed_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3480F4-3BB9-4DA3-91BB-A78FE937C53E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C2726B-0AF0-4503-8BB8-139790EE6A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>Number of Shares:</t>
   </si>
   <si>
-    <t>Next Earnings Date:</t>
-  </si>
-  <si>
     <t>Capitalization:</t>
   </si>
   <si>
@@ -397,9 +394,6 @@
   </si>
   <si>
     <t xml:space="preserve">PB = </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Inputs</t>
   </si>
   <si>
     <t>Assets</t>
@@ -1341,12 +1335,18 @@
   <si>
     <t>Type:</t>
   </si>
+  <si>
+    <t>Most Recent Quarter Inputs</t>
+  </si>
+  <si>
+    <t>Next Review Date:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="24">
+  <numFmts count="25">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1371,8 +1371,9 @@
     <numFmt numFmtId="182" formatCode="&quot;Discount rate = &quot;0.00%"/>
     <numFmt numFmtId="183" formatCode="#,##0.00;[Red]#,##0.00"/>
     <numFmt numFmtId="184" formatCode="[$-409]mmm\-yy;@"/>
+    <numFmt numFmtId="187" formatCode="&quot;in&quot;\ 0\ &quot;Months&quot;"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1578,6 +1579,12 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="26">
     <fill>
@@ -1731,7 +1738,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="98">
+  <borders count="101">
     <border>
       <left/>
       <right/>
@@ -2968,13 +2975,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="dotted">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="446">
+  <cellXfs count="452">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3871,154 +3919,18 @@
     <xf numFmtId="177" fontId="2" fillId="18" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="11" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="4" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="11" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="11" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="4" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="4" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="3" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="2" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4027,6 +3939,9 @@
     </xf>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="6" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4038,11 +3953,141 @@
     <xf numFmtId="0" fontId="7" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="4" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="11" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="11" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="4" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="4" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4064,7 +4109,6 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4088,7 +4132,31 @@
     <xf numFmtId="4" fontId="5" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="179" fontId="30" fillId="10" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="2" fillId="10" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="98" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4197,8 +4265,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0000FF"/>
       <color rgb="FFFFFFCC"/>
-      <color rgb="FF0000FF"/>
       <color rgb="FFB6D7A8"/>
       <color rgb="FFCCFF33"/>
     </mruColors>
@@ -4419,7 +4487,7 @@
   <dimension ref="A1:L967"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:J21"/>
+      <selection activeCell="I6" sqref="I6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4447,11 +4515,11 @@
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="358" t="str">
+      <c r="C2" s="403" t="str">
         <f>C3&amp;" : "&amp;C4</f>
         <v>0683.HK : KERRY PPT</v>
       </c>
-      <c r="D2" s="359"/>
+      <c r="D2" s="404"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
@@ -4463,27 +4531,27 @@
       <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="360" t="s">
-        <v>342</v>
-      </c>
-      <c r="D3" s="361"/>
+      <c r="C3" s="405" t="s">
+        <v>340</v>
+      </c>
+      <c r="D3" s="406"/>
       <c r="E3" s="15"/>
       <c r="G3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="373" t="s">
+      <c r="I3" s="413" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="374"/>
+      <c r="J3" s="414"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="362" t="s">
-        <v>343</v>
-      </c>
-      <c r="D4" s="363"/>
+      <c r="C4" s="407" t="s">
+        <v>341</v>
+      </c>
+      <c r="D4" s="408"/>
       <c r="E4" s="6"/>
       <c r="G4" s="5" t="s">
         <v>5</v>
@@ -4500,10 +4568,10 @@
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="364">
+      <c r="C5" s="409">
         <v>44956</v>
       </c>
-      <c r="D5" s="363"/>
+      <c r="D5" s="408"/>
       <c r="E5" s="158" t="str">
         <f ca="1">IF(C5+30&gt;=TODAY(),"Patience Premium","")</f>
         <v>Patience Premium</v>
@@ -4511,36 +4579,39 @@
       <c r="G5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="375">
+      <c r="I5" s="393">
         <v>1451309952</v>
       </c>
-      <c r="J5" s="376"/>
+      <c r="J5" s="394"/>
       <c r="K5" s="195"/>
       <c r="L5" s="113"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="367">
-        <v>45001</v>
-      </c>
-      <c r="D6" s="368"/>
+        <v>355</v>
+      </c>
+      <c r="C6" s="448">
+        <v>8</v>
+      </c>
+      <c r="D6" s="449">
+        <f>EOMONTH(EDATE('Asset Model'!D9,C6),0)</f>
+        <v>44985</v>
+      </c>
       <c r="E6" s="158"/>
       <c r="G6" s="171" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" s="170"/>
-      <c r="I6" s="377">
+      <c r="I6" s="415">
         <f>I4*I5/1000000</f>
         <v>28793.98944768</v>
       </c>
-      <c r="J6" s="378"/>
+      <c r="J6" s="416"/>
       <c r="K6" s="195"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="176" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="184">
         <f>(Data!C40)/I4</f>
@@ -4557,7 +4628,7 @@
       <c r="C8" s="128"/>
       <c r="E8" s="6"/>
       <c r="G8" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H8" s="169"/>
       <c r="I8" s="6"/>
@@ -4565,12 +4636,12 @@
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="5"/>
       <c r="G9" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I9" s="157">
         <f>IF(Data!F3&lt;=0,"NNI",I4/((Data!F3*I12)/(I5/Data!C4)))</f>
@@ -4583,17 +4654,17 @@
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="186" t="s">
         <v>15</v>
-      </c>
-      <c r="C10" s="186" t="s">
-        <v>16</v>
       </c>
       <c r="D10" s="161">
         <v>2.9100000000000001E-2</v>
       </c>
       <c r="E10" s="5"/>
       <c r="G10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I10" s="175">
         <f>I4/(Data!C28*I12*Data!C4/Common_Shares)</f>
@@ -4606,7 +4677,7 @@
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C11" s="263">
         <v>0.1</v>
@@ -4617,17 +4688,17 @@
       </c>
       <c r="E11" s="13"/>
       <c r="G11" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H11" s="6"/>
-      <c r="I11" s="385" t="s">
+      <c r="I11" s="423" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="386"/>
+      <c r="J11" s="424"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="103" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C12" s="352">
         <v>2.9100000000000001E-2</v>
@@ -4637,7 +4708,7 @@
         <v>0.19354444444444446</v>
       </c>
       <c r="G12" s="171" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H12" s="170"/>
       <c r="I12" s="172">
@@ -4652,24 +4723,24 @@
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="164" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D14" s="233">
         <f ca="1">'FCFF Model'!C33</f>
         <v>19.213458639736121</v>
       </c>
       <c r="E14" s="164" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F14" s="233">
         <f ca="1">'FCFF Model'!E33</f>
         <v>21.121184119130799</v>
       </c>
       <c r="G14" s="234" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H14" s="245">
         <f ca="1">IF('FCFF Model'!C36&lt;0, "Error", 'FCFF Model'!C36)</f>
@@ -4682,23 +4753,23 @@
       <c r="A15" s="6"/>
       <c r="B15" s="128"/>
       <c r="C15" s="312" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D15" s="120" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="120" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="120" t="s">
+      <c r="F15" s="120" t="s">
         <v>23</v>
-      </c>
-      <c r="F15" s="120" t="s">
-        <v>24</v>
       </c>
       <c r="G15" s="176"/>
       <c r="H15" s="85" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J15" s="165" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4706,7 +4777,7 @@
         <f>I4</f>
         <v>19.84</v>
       </c>
-      <c r="C16" s="414">
+      <c r="C16" s="364">
         <f ca="1">D11/2</f>
         <v>8.2222222222222224E-2</v>
       </c>
@@ -4714,7 +4785,7 @@
         <f ca="1">H14/B16-1-C16</f>
         <v>-6.4911970852888717E-2</v>
       </c>
-      <c r="E16" s="395">
+      <c r="E16" s="400">
         <f>'FCFF Model'!D14</f>
         <v>0.95</v>
       </c>
@@ -4722,15 +4793,15 @@
         <f>E16/B16</f>
         <v>4.7883064516129031E-2</v>
       </c>
-      <c r="G16" s="382" t="s">
-        <v>28</v>
-      </c>
-      <c r="H16" s="379">
+      <c r="G16" s="420" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="417">
         <f>('FCFF Model'!G21)*Exchange_Rate</f>
         <v>15.381471906974147</v>
       </c>
-      <c r="I16" s="382" t="s">
-        <v>29</v>
+      <c r="I16" s="420" t="s">
+        <v>28</v>
       </c>
       <c r="J16" s="266">
         <f>B16-$H$16</f>
@@ -4741,19 +4812,19 @@
       <c r="B17" s="202">
         <v>18.5</v>
       </c>
-      <c r="C17" s="415"/>
+      <c r="C17" s="365"/>
       <c r="D17" s="206">
         <f ca="1">H14/B17-1-C16</f>
         <v>8.77428519224141E-3</v>
       </c>
-      <c r="E17" s="396"/>
+      <c r="E17" s="401"/>
       <c r="F17" s="209">
         <f>E16/B17</f>
         <v>5.1351351351351347E-2</v>
       </c>
-      <c r="G17" s="383"/>
-      <c r="H17" s="380"/>
-      <c r="I17" s="383"/>
+      <c r="G17" s="421"/>
+      <c r="H17" s="418"/>
+      <c r="I17" s="421"/>
       <c r="J17" s="265">
         <f>B17-$H$16</f>
         <v>3.1185280930258532</v>
@@ -4763,19 +4834,19 @@
       <c r="B18" s="203">
         <v>18</v>
       </c>
-      <c r="C18" s="416"/>
+      <c r="C18" s="366"/>
       <c r="D18" s="207">
         <f ca="1">H14/B18-1-C16</f>
         <v>3.9079743731531974E-2</v>
       </c>
-      <c r="E18" s="397"/>
+      <c r="E18" s="402"/>
       <c r="F18" s="210">
         <f>E16/B18</f>
         <v>5.2777777777777778E-2</v>
       </c>
-      <c r="G18" s="384"/>
-      <c r="H18" s="381"/>
-      <c r="I18" s="384"/>
+      <c r="G18" s="422"/>
+      <c r="H18" s="419"/>
+      <c r="I18" s="422"/>
       <c r="J18" s="267">
         <f>B18-$H$16</f>
         <v>2.6185280930258532</v>
@@ -4788,13 +4859,13 @@
     <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="D20" s="445"/>
-      <c r="E20" s="445"/>
+        <v>353</v>
+      </c>
+      <c r="D20" s="450"/>
+      <c r="E20" s="451"/>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
@@ -4804,54 +4875,54 @@
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="369" t="s">
-        <v>335</v>
-      </c>
-      <c r="D21" s="370"/>
-      <c r="E21" s="370"/>
-      <c r="F21" s="370"/>
-      <c r="G21" s="370"/>
-      <c r="H21" s="370"/>
-      <c r="I21" s="370"/>
-      <c r="J21" s="371"/>
+        <v>30</v>
+      </c>
+      <c r="C21" s="410" t="s">
+        <v>333</v>
+      </c>
+      <c r="D21" s="411"/>
+      <c r="E21" s="411"/>
+      <c r="F21" s="411"/>
+      <c r="G21" s="411"/>
+      <c r="H21" s="411"/>
+      <c r="I21" s="411"/>
+      <c r="J21" s="412"/>
     </row>
     <row r="22" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="387" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="358" t="s">
+        <v>349</v>
+      </c>
+      <c r="D22" s="359"/>
+      <c r="E22" s="359"/>
+      <c r="F22" s="359"/>
+      <c r="G22" s="358" t="s">
         <v>351</v>
       </c>
-      <c r="D22" s="388"/>
-      <c r="E22" s="388"/>
-      <c r="F22" s="388"/>
-      <c r="G22" s="387" t="s">
-        <v>353</v>
-      </c>
-      <c r="H22" s="387"/>
-      <c r="I22" s="388"/>
-      <c r="J22" s="388"/>
+      <c r="H22" s="358"/>
+      <c r="I22" s="359"/>
+      <c r="J22" s="359"/>
     </row>
     <row r="23" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="372" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="360" t="s">
+        <v>348</v>
+      </c>
+      <c r="D23" s="361"/>
+      <c r="E23" s="361"/>
+      <c r="F23" s="361"/>
+      <c r="G23" s="360" t="s">
         <v>350</v>
       </c>
-      <c r="D23" s="368"/>
-      <c r="E23" s="368"/>
-      <c r="F23" s="368"/>
-      <c r="G23" s="372" t="s">
-        <v>352</v>
-      </c>
-      <c r="H23" s="372"/>
-      <c r="I23" s="368"/>
-      <c r="J23" s="368"/>
+      <c r="H23" s="360"/>
+      <c r="I23" s="361"/>
+      <c r="J23" s="361"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6"/>
@@ -4867,10 +4938,10 @@
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="23" t="s">
         <v>34</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>35</v>
       </c>
       <c r="D25" s="36">
         <v>600000</v>
@@ -4884,157 +4955,157 @@
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="362"/>
+      <c r="D26" s="363"/>
+      <c r="E26" s="362"/>
+      <c r="F26" s="363"/>
+      <c r="G26" s="382"/>
+      <c r="H26" s="383"/>
+      <c r="I26" s="397" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="365"/>
-      <c r="D26" s="366"/>
-      <c r="E26" s="365"/>
-      <c r="F26" s="366"/>
-      <c r="G26" s="399"/>
-      <c r="H26" s="400"/>
-      <c r="I26" s="413" t="s">
-        <v>37</v>
-      </c>
-      <c r="J26" s="413"/>
+      <c r="J26" s="397"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="394">
+        <v>37</v>
+      </c>
+      <c r="C27" s="399">
         <f>C31/D25</f>
         <v>0</v>
       </c>
-      <c r="D27" s="393"/>
-      <c r="E27" s="392">
+      <c r="D27" s="379"/>
+      <c r="E27" s="398">
         <f>E31/D25</f>
         <v>0</v>
       </c>
-      <c r="F27" s="393"/>
-      <c r="G27" s="401">
+      <c r="F27" s="379"/>
+      <c r="G27" s="384">
         <f>G31/D25</f>
         <v>0</v>
       </c>
-      <c r="H27" s="402"/>
-      <c r="I27" s="404">
+      <c r="H27" s="385"/>
+      <c r="I27" s="386">
         <f>C27+E27+G27</f>
         <v>0</v>
       </c>
-      <c r="J27" s="404"/>
+      <c r="J27" s="386"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="391"/>
-      <c r="D28" s="388"/>
-      <c r="E28" s="391"/>
-      <c r="F28" s="388"/>
-      <c r="G28" s="375"/>
-      <c r="H28" s="376"/>
-      <c r="I28" s="418">
+        <v>38</v>
+      </c>
+      <c r="C28" s="380"/>
+      <c r="D28" s="359"/>
+      <c r="E28" s="380"/>
+      <c r="F28" s="359"/>
+      <c r="G28" s="393"/>
+      <c r="H28" s="394"/>
+      <c r="I28" s="369">
         <f>C28+E28+G28</f>
         <v>0</v>
       </c>
-      <c r="J28" s="418"/>
+      <c r="J28" s="369"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="398"/>
-      <c r="D29" s="388"/>
-      <c r="E29" s="398"/>
-      <c r="F29" s="388"/>
-      <c r="G29" s="405"/>
-      <c r="H29" s="406"/>
-      <c r="I29" s="411"/>
-      <c r="J29" s="411"/>
+        <v>39</v>
+      </c>
+      <c r="C29" s="381"/>
+      <c r="D29" s="359"/>
+      <c r="E29" s="381"/>
+      <c r="F29" s="359"/>
+      <c r="G29" s="387"/>
+      <c r="H29" s="388"/>
+      <c r="I29" s="395"/>
+      <c r="J29" s="395"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="389">
+        <v>40</v>
+      </c>
+      <c r="C30" s="367">
         <f>C29*$I$5/1000000</f>
         <v>0</v>
       </c>
-      <c r="D30" s="390"/>
-      <c r="E30" s="389">
+      <c r="D30" s="374"/>
+      <c r="E30" s="367">
         <f>E29*$I$5/1000000</f>
         <v>0</v>
       </c>
-      <c r="F30" s="390"/>
-      <c r="G30" s="407">
+      <c r="F30" s="374"/>
+      <c r="G30" s="389">
         <f>G29*$I$5/1000000</f>
         <v>0</v>
       </c>
-      <c r="H30" s="408"/>
-      <c r="I30" s="412"/>
-      <c r="J30" s="412"/>
+      <c r="H30" s="390"/>
+      <c r="I30" s="396"/>
+      <c r="J30" s="396"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="423">
+        <v>41</v>
+      </c>
+      <c r="C31" s="375">
         <f>C28*C29</f>
         <v>0</v>
       </c>
-      <c r="D31" s="424"/>
-      <c r="E31" s="417">
+      <c r="D31" s="376"/>
+      <c r="E31" s="368">
         <f>E28*E29</f>
         <v>0</v>
       </c>
-      <c r="F31" s="425"/>
-      <c r="G31" s="409">
+      <c r="F31" s="377"/>
+      <c r="G31" s="391">
         <f>G28*G29</f>
         <v>0</v>
       </c>
-      <c r="H31" s="410"/>
-      <c r="I31" s="417">
+      <c r="H31" s="392"/>
+      <c r="I31" s="368">
         <f>C31+E31+G31</f>
         <v>0</v>
       </c>
-      <c r="J31" s="417"/>
+      <c r="J31" s="368"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="419"/>
-      <c r="D32" s="420"/>
-      <c r="E32" s="403" t="str">
+        <v>42</v>
+      </c>
+      <c r="C32" s="370"/>
+      <c r="D32" s="371"/>
+      <c r="E32" s="378" t="str">
         <f>IF(C31=0,"-",(C31+E31)/(C28+E28))</f>
         <v>-</v>
       </c>
-      <c r="F32" s="393"/>
+      <c r="F32" s="379"/>
       <c r="G32" s="153"/>
       <c r="H32" s="153"/>
-      <c r="I32" s="403" t="str">
+      <c r="I32" s="378" t="str">
         <f>IF(I31=0,"",I31/I28)</f>
         <v/>
       </c>
-      <c r="J32" s="403"/>
+      <c r="J32" s="378"/>
     </row>
     <row r="33" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="421"/>
-      <c r="D33" s="422"/>
-      <c r="E33" s="389" t="str">
+        <v>43</v>
+      </c>
+      <c r="C33" s="372"/>
+      <c r="D33" s="373"/>
+      <c r="E33" s="367" t="str">
         <f>IF(E32="-","-",E32*$I$5/1000000)</f>
         <v>-</v>
       </c>
-      <c r="F33" s="390"/>
+      <c r="F33" s="374"/>
       <c r="G33" s="154"/>
       <c r="H33" s="154"/>
-      <c r="I33" s="389" t="str">
+      <c r="I33" s="367" t="str">
         <f>IF(I32="","",I32*$I$5/1000000)</f>
         <v/>
       </c>
-      <c r="J33" s="389"/>
+      <c r="J33" s="367"/>
     </row>
     <row r="34" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5972,6 +6043,39 @@
     <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C21:J21"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I26:J26"/>
     <mergeCell ref="G22:J22"/>
     <mergeCell ref="G23:J23"/>
     <mergeCell ref="E26:F26"/>
@@ -5988,39 +6092,6 @@
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C21:J21"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="C22:F22"/>
   </mergeCells>
   <conditionalFormatting sqref="I16">
     <cfRule type="cellIs" dxfId="10" priority="19" operator="lessThan">
@@ -6071,7 +6142,7 @@
   <dimension ref="A1:N964"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6093,7 +6164,7 @@
     <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="41"/>
       <c r="B2" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="42"/>
       <c r="D2" s="42"/>
@@ -6110,7 +6181,7 @@
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="192">
         <v>44561</v>
@@ -6134,7 +6205,7 @@
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="37">
         <v>1000</v>
@@ -6210,7 +6281,7 @@
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="37">
         <v>15326764</v>
@@ -6234,7 +6305,7 @@
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="14">
         <f t="shared" ref="C8:L8" si="0">IF(D7="","",C7/D7-1)</f>
@@ -6282,7 +6353,7 @@
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="37">
         <v>6583757</v>
@@ -6306,7 +6377,7 @@
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="14">
         <f t="shared" ref="C10:M10" si="1">IF(C7="","",(C7-C9)/C7)</f>
@@ -6357,7 +6428,7 @@
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="37">
         <v>2003343</v>
@@ -6381,7 +6452,7 @@
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="14">
         <f t="shared" ref="C12:M12" si="2">IF(C7="","",C10-C13)</f>
@@ -6432,7 +6503,7 @@
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="14">
         <f t="shared" ref="C13:M13" si="3">IF(C14="","",C14/C7)</f>
@@ -6483,7 +6554,7 @@
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="29">
         <f t="shared" ref="C14:M14" si="4">IF(C7="","",C7-C9-C11)</f>
@@ -6534,7 +6605,7 @@
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="14">
         <f>IF(D14="","",IF(ABS(C14+D14)=ABS(C14)+ABS(D14),IF(C14&lt;0,-1,1)*(C14-D14)/D14,"Turn"))</f>
@@ -6585,7 +6656,7 @@
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="182">
         <f>IF(C14="","",C14*(1-'FCFF Model'!$D$6))</f>
@@ -6636,7 +6707,7 @@
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" s="181" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="166">
         <f t="shared" ref="C17:M17" si="6">IF(C7="","",C16/C7)</f>
@@ -6687,7 +6758,7 @@
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="37">
         <v>10358011</v>
@@ -6711,7 +6782,7 @@
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="14">
         <f t="shared" ref="C19:M19" si="7">IF(C7="","",C18/C7)</f>
@@ -6762,7 +6833,7 @@
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
       <c r="B20" s="48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="49">
         <f>'Asset Model'!C26</f>
@@ -6787,7 +6858,7 @@
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" s="48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C21" s="224">
         <v>20068482</v>
@@ -6811,7 +6882,7 @@
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="B22" s="48" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C22" s="224">
         <v>67022531</v>
@@ -6831,7 +6902,7 @@
     <row r="23" spans="1:14" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
       <c r="B23" s="48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="49">
         <f>'Asset Model'!I11+'Asset Model'!I12+'Asset Model'!I13</f>
@@ -6856,7 +6927,7 @@
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
       <c r="B24" s="180" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C24" s="177">
         <f>'Asset Model'!I12</f>
@@ -6881,7 +6952,7 @@
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
       <c r="B25" s="48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="49">
         <f>'Asset Model'!I28+'Asset Model'!I29+'Asset Model'!I30</f>
@@ -6906,7 +6977,7 @@
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="180" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="179">
         <f>'Asset Model'!I29</f>
@@ -6931,7 +7002,7 @@
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="48" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C27" s="29">
         <f t="shared" ref="C27:M27" si="8">IF(C7="","",C23+C25)</f>
@@ -6982,7 +7053,7 @@
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9"/>
       <c r="B28" s="48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" s="224">
         <v>128099808</v>
@@ -7006,7 +7077,7 @@
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9"/>
       <c r="B29" s="180" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C29" s="223">
         <v>157397300.09900001</v>
@@ -7026,7 +7097,7 @@
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9"/>
       <c r="B30" s="48" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C30" s="49">
         <f>'Asset Model'!C59</f>
@@ -7051,7 +7122,7 @@
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9"/>
       <c r="B31" s="48" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C31" s="183">
         <v>562656</v>
@@ -7075,7 +7146,7 @@
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>
       <c r="B32" s="48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" s="49">
         <f>'Asset Model'!C36+'Asset Model'!C37+'Asset Model'!C38</f>
@@ -7100,7 +7171,7 @@
     <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
       <c r="B33" s="48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33" s="14">
         <f t="shared" ref="C33:M33" si="9">IF(D7="","",(C32-D32)/C32)</f>
@@ -7151,7 +7222,7 @@
     <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
       <c r="B34" s="48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C34" s="329">
         <f t="shared" ref="C34:M34" si="10">IF(D7="","",(C7-D7)*$D$50)</f>
@@ -7202,7 +7273,7 @@
     <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
       <c r="B35" s="48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" s="182">
         <f t="shared" ref="C35:M35" si="11">IF(D7="","",C32-D32+C34)</f>
@@ -7253,7 +7324,7 @@
     <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="328" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C36" s="319">
         <f t="shared" ref="C36:M36" si="12">IF(C35="","",C35/C16)</f>
@@ -7304,7 +7375,7 @@
     <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -7322,7 +7393,7 @@
     <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
       <c r="B38" s="216" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C38" s="213">
         <v>5316230</v>
@@ -7346,7 +7417,7 @@
     <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9"/>
       <c r="B39" s="181" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C39" s="212">
         <v>40396</v>
@@ -7370,7 +7441,7 @@
     <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9"/>
       <c r="B40" s="181" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C40" s="218">
         <f t="shared" ref="C40:M40" si="13">IF(C38="","",C38*$C$4/Common_Shares)</f>
@@ -7421,7 +7492,7 @@
     <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9"/>
       <c r="B41" s="217" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C41" s="220">
         <f t="shared" ref="C41:M41" si="14">IF(C39="","",C39*$C$4/Common_Shares)</f>
@@ -7472,7 +7543,7 @@
     <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="9"/>
       <c r="B42" s="120" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
@@ -7489,7 +7560,7 @@
     <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="9"/>
       <c r="B43" s="47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C43" s="52">
         <f>IF(C29="","",C25/C28)</f>
@@ -7540,7 +7611,7 @@
     <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="9"/>
       <c r="B44" s="48" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C44" s="14">
         <f>IF(C29="","",C27/C29)</f>
@@ -7591,7 +7662,7 @@
     <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="9"/>
       <c r="B45" s="48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C45" s="54">
         <f t="shared" ref="C45:M45" si="17">IF(C14="","",IF(C27&lt;=0,"-",C14/C27))</f>
@@ -7642,7 +7713,7 @@
     <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="9"/>
       <c r="B46" s="48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C46" s="14">
         <f t="shared" ref="C46:M46" si="18">IF(C16="","",IF(C31&lt;=0,"-",C31/C16))</f>
@@ -7693,7 +7764,7 @@
     <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="9"/>
       <c r="B47" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C47" s="55">
         <f>IF(C20="","",C20/C21)</f>
@@ -7758,7 +7829,7 @@
     <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="9"/>
       <c r="B49" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C49" s="56"/>
       <c r="D49" s="56"/>
@@ -7768,27 +7839,27 @@
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="9"/>
       <c r="B50" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C50" s="6"/>
-      <c r="D50" s="431">
+      <c r="D50" s="430">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="E50" s="432"/>
+      <c r="E50" s="431"/>
       <c r="F50" s="354" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="9"/>
       <c r="B51" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="425" t="s">
         <v>84</v>
       </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="426" t="s">
-        <v>85</v>
-      </c>
-      <c r="E51" s="388"/>
+      <c r="E51" s="359"/>
       <c r="F51" s="6"/>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -7800,29 +7871,29 @@
     <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="9"/>
       <c r="B53" s="58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C53" s="59"/>
-      <c r="D53" s="427">
+      <c r="D53" s="426">
         <v>5</v>
       </c>
-      <c r="E53" s="428"/>
+      <c r="E53" s="427"/>
       <c r="F53" s="60"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9"/>
       <c r="B54" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="C54" s="62" t="s">
+      <c r="D54" s="428" t="s">
         <v>88</v>
       </c>
-      <c r="D54" s="429" t="s">
+      <c r="E54" s="429"/>
+      <c r="F54" s="63" t="s">
         <v>89</v>
-      </c>
-      <c r="E54" s="430"/>
-      <c r="F54" s="63" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -8047,7 +8118,7 @@
     <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="9"/>
       <c r="B66" s="70" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C66" s="57"/>
       <c r="D66" s="57"/>
@@ -8060,7 +8131,7 @@
     <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="9"/>
       <c r="B67" s="70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C67" s="57"/>
       <c r="D67" s="57"/>
@@ -8082,22 +8153,22 @@
       <c r="A69" s="9"/>
       <c r="B69" s="72"/>
       <c r="C69" s="73" t="s">
+        <v>92</v>
+      </c>
+      <c r="D69" s="73" t="s">
         <v>93</v>
       </c>
-      <c r="D69" s="73" t="s">
+      <c r="E69" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="E69" s="74" t="s">
+      <c r="F69" s="75" t="s">
         <v>95</v>
-      </c>
-      <c r="F69" s="75" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="9"/>
       <c r="B70" s="70" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C70" s="76">
         <f>C14</f>
@@ -8108,16 +8179,16 @@
         <v>6739664</v>
       </c>
       <c r="E70" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="F70" s="71" t="s">
         <v>98</v>
-      </c>
-      <c r="F70" s="71" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="9"/>
       <c r="B71" s="70" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C71" s="77">
         <f t="shared" ref="C71:D71" si="24">C70/$C$7</f>
@@ -8128,16 +8199,16 @@
         <v>0.4397317007034231</v>
       </c>
       <c r="E71" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="F71" s="71" t="s">
         <v>101</v>
-      </c>
-      <c r="F71" s="71" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="9"/>
       <c r="B72" s="70" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C72" s="76">
         <f>C35</f>
@@ -8148,16 +8219,16 @@
         <v>2130419.6779999998</v>
       </c>
       <c r="E72" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="F72" s="71" t="s">
         <v>104</v>
-      </c>
-      <c r="F72" s="71" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="9"/>
       <c r="B73" s="70" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C73" s="76">
         <f>C16</f>
@@ -8168,16 +8239,16 @@
         <v>5627619.4399999995</v>
       </c>
       <c r="E73" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="F73" s="71" t="s">
         <v>107</v>
-      </c>
-      <c r="F73" s="71" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="9"/>
       <c r="B74" s="70" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C74" s="76">
         <f>F3</f>
@@ -8188,16 +8259,16 @@
         <v>10358011</v>
       </c>
       <c r="E74" s="57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F74" s="71" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="9"/>
       <c r="B75" s="78" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C75" s="79" t="e">
         <f>#REF!</f>
@@ -8208,10 +8279,10 @@
         <v>#REF!</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F75" s="80" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -9587,8 +9658,8 @@
   </sheetPr>
   <dimension ref="A2:J61"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9604,11 +9675,11 @@
   <sheetData>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="435" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" s="435"/>
-      <c r="D2" s="435"/>
+      <c r="B2" s="444" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="444"/>
+      <c r="D2" s="443"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
@@ -9617,7 +9688,7 @@
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="225">
@@ -9631,7 +9702,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="85" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I3" s="122">
         <f>((D3-D4)*Dashboard!I12*Data!C4)/Dashboard!I5</f>
@@ -9640,7 +9711,7 @@
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="194">
@@ -9655,13 +9726,13 @@
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D5" s="6"/>
       <c r="E5" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="83" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="84">
@@ -9675,7 +9746,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="85" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I6" s="28">
         <f>IF(Data!F3&lt;=0,"NNI",D7/((Data!F3*Dashboard!I12)/(Dashboard!I5/Data!C4)))</f>
@@ -9685,7 +9756,7 @@
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" s="86">
         <f>MAX((D6*Dashboard!I12*Data!C4)/Dashboard!I5, 0)</f>
@@ -9693,7 +9764,7 @@
       </c>
       <c r="E7" s="87"/>
       <c r="H7" s="85" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I7" s="28">
         <f>D7/(Data!C28*Dashboard!I12*Data!C4/Common_Shares)</f>
@@ -9705,43 +9776,48 @@
       <c r="D8" s="6"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
-      <c r="B9" s="435" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9" s="435"/>
-      <c r="D9" s="435"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="B9" s="445" t="s">
+        <v>354</v>
+      </c>
+      <c r="C9" s="336"/>
+      <c r="D9" s="446">
+        <v>44742</v>
+      </c>
+      <c r="E9" s="447" t="str">
+        <f>IF(D9=Data!C3,"FY","Quarter")</f>
+        <v>Quarter</v>
+      </c>
+      <c r="F9" s="170"/>
+      <c r="G9" s="170"/>
+      <c r="H9" s="170"/>
+      <c r="I9" s="170"/>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="E10" s="24" t="s">
         <v>123</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>125</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="88" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C11" s="89">
         <v>16946370</v>
@@ -9756,7 +9832,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I11" s="89">
         <v>2253528</v>
@@ -9765,7 +9841,7 @@
     </row>
     <row r="12" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C12" s="89">
         <v>0</v>
@@ -9780,7 +9856,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I12" s="89">
         <v>31180.352999999999</v>
@@ -9789,7 +9865,7 @@
     </row>
     <row r="13" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C13" s="89">
         <v>0</v>
@@ -9804,7 +9880,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I13" s="89">
         <v>861793.34100000001</v>
@@ -9813,7 +9889,7 @@
     </row>
     <row r="14" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C14" s="89">
         <v>0</v>
@@ -9828,7 +9904,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I14" s="89">
         <v>0</v>
@@ -9837,7 +9913,7 @@
     </row>
     <row r="15" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C15" s="89">
         <v>0</v>
@@ -9852,7 +9928,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I15" s="199">
         <f>I26-SUM(I11:I14)</f>
@@ -9862,7 +9938,7 @@
     </row>
     <row r="16" spans="1:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C16" s="89">
         <v>0</v>
@@ -9882,7 +9958,7 @@
     </row>
     <row r="17" spans="2:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C17" s="89">
         <v>2617395</v>
@@ -9902,7 +9978,7 @@
     </row>
     <row r="18" spans="2:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C18" s="89">
         <v>0</v>
@@ -9915,13 +9991,13 @@
         <v>0</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="2:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C19" s="89">
         <v>17196881</v>
@@ -9934,7 +10010,7 @@
         <v>10318128.6</v>
       </c>
       <c r="F19" s="264" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G19" s="125">
         <f>IF(F19="Y",0,1)</f>
@@ -9945,7 +10021,7 @@
     </row>
     <row r="20" spans="2:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C20" s="89">
         <v>20570771</v>
@@ -9958,7 +10034,7 @@
         <v>8228308.4000000004</v>
       </c>
       <c r="F20" s="264" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G20" s="125">
         <f>IF(F20="Y",0,1)</f>
@@ -9969,7 +10045,7 @@
     </row>
     <row r="21" spans="2:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C21" s="89">
         <v>634405</v>
@@ -9988,7 +10064,7 @@
     </row>
     <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C22" s="89">
         <v>0</v>
@@ -10010,7 +10086,7 @@
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="91" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C24" s="95">
         <f>SUM(C11:C14)</f>
@@ -10027,7 +10103,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="91" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I24" s="94">
         <f>E24/($I$26-I13)</f>
@@ -10040,7 +10116,7 @@
     </row>
     <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="91" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C25" s="95">
         <f>C24+SUM(C15:C17)</f>
@@ -10057,7 +10133,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="91" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I25" s="94">
         <f>E25/$I$26</f>
@@ -10067,7 +10143,7 @@
     </row>
     <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C26" s="95">
         <f>SUM(C11:C22)</f>
@@ -10082,7 +10158,7 @@
         <v>37404189.25</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I26" s="199">
         <f>Data!C21</f>
@@ -10100,7 +10176,7 @@
     </row>
     <row r="28" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C28" s="89">
         <v>0</v>
@@ -10114,7 +10190,7 @@
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I28" s="89">
         <f>996632.901+1804212.761+142405.676</f>
@@ -10124,7 +10200,7 @@
     </row>
     <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C29" s="89">
         <v>2179420</v>
@@ -10139,7 +10215,7 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I29" s="89">
         <v>13550.745000000001</v>
@@ -10148,7 +10224,7 @@
     </row>
     <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C30" s="89">
         <v>608531</v>
@@ -10163,7 +10239,7 @@
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I30" s="89">
         <v>0</v>
@@ -10172,7 +10248,7 @@
     </row>
     <row r="31" spans="2:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C31" s="89">
         <v>0</v>
@@ -10187,7 +10263,7 @@
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I31" s="89">
         <v>0</v>
@@ -10196,7 +10272,7 @@
     </row>
     <row r="32" spans="2:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C32" s="89">
         <v>1107494</v>
@@ -10209,11 +10285,11 @@
         <v>442997.60000000003</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I32" s="199">
         <f>I42-SUM(I28:I31)</f>
@@ -10223,7 +10299,7 @@
     </row>
     <row r="33" spans="2:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C33" s="89">
         <v>27509451</v>
@@ -10236,7 +10312,7 @@
         <v>11003780.4</v>
       </c>
       <c r="F33" s="264" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G33" s="125">
         <f>IF(F33="Y",0,1)</f>
@@ -10246,7 +10322,7 @@
     </row>
     <row r="34" spans="2:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C34" s="89">
         <v>80948092</v>
@@ -10259,7 +10335,7 @@
         <v>48568855.199999996</v>
       </c>
       <c r="F34" s="264" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G34" s="125">
         <f>IF(F34="Y",0,1)</f>
@@ -10268,7 +10344,7 @@
     </row>
     <row r="35" spans="2:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C35" s="89">
         <v>21257867</v>
@@ -10281,7 +10357,7 @@
         <v>8503146.8000000007</v>
       </c>
       <c r="F35" s="264" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G35" s="125">
         <f>IF(F35="Y",0,1)</f>
@@ -10290,7 +10366,7 @@
     </row>
     <row r="36" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C36" s="89">
         <v>21664879</v>
@@ -10307,7 +10383,7 @@
     </row>
     <row r="37" spans="2:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C37" s="89">
         <v>1826761</v>
@@ -10324,7 +10400,7 @@
     </row>
     <row r="38" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C38" s="89">
         <v>122504</v>
@@ -10341,7 +10417,7 @@
     </row>
     <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C39" s="89">
         <v>0</v>
@@ -10358,7 +10434,7 @@
     </row>
     <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C40" s="89">
         <v>0</v>
@@ -10381,7 +10457,7 @@
     </row>
     <row r="42" spans="2:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C42" s="92">
         <f>SUM(C28:C40)</f>
@@ -10398,7 +10474,7 @@
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
       <c r="H42" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I42" s="199">
         <f>Data!C22</f>
@@ -10414,7 +10490,7 @@
     </row>
     <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="91" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C44" s="95">
         <f>C24+SUM(C28:C29)</f>
@@ -10431,7 +10507,7 @@
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="91" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I44" s="94">
         <f>E44/$I$46</f>
@@ -10444,7 +10520,7 @@
     </row>
     <row r="45" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="91" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C45" s="95">
         <f>C44+(C25-C24)+SUM(C30:C33)</f>
@@ -10461,7 +10537,7 @@
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="91" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I45" s="94">
         <f>E45/$I$46</f>
@@ -10471,7 +10547,7 @@
     </row>
     <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C46" s="95">
         <f>C26+C42</f>
@@ -10488,7 +10564,7 @@
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I46" s="199">
         <f>I26+I42</f>
@@ -10504,14 +10580,14 @@
     </row>
     <row r="48" spans="2:10" ht="14" x14ac:dyDescent="0.3">
       <c r="B48" s="22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C48" s="22"/>
       <c r="D48" s="56"/>
     </row>
     <row r="49" spans="2:9" ht="14" x14ac:dyDescent="0.3">
       <c r="B49" s="277" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C49" s="6"/>
       <c r="D49" s="278" t="str">
@@ -10522,7 +10598,7 @@
     </row>
     <row r="50" spans="2:9" ht="14" x14ac:dyDescent="0.3">
       <c r="B50" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C50" s="279">
         <f>D4</f>
@@ -10545,55 +10621,55 @@
     </row>
     <row r="52" spans="2:9" ht="14" x14ac:dyDescent="0.3">
       <c r="B52" s="100" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C52" s="5"/>
-      <c r="D52" s="418">
+      <c r="D52" s="369">
         <f>D53+D54+D55</f>
         <v>6103303.7770000007</v>
       </c>
-      <c r="E52" s="437"/>
+      <c r="E52" s="435"/>
       <c r="F52" s="57"/>
       <c r="G52" s="57"/>
     </row>
     <row r="53" spans="2:9" ht="14" x14ac:dyDescent="0.3">
       <c r="B53" s="83" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C53" s="6"/>
-      <c r="D53" s="418">
+      <c r="D53" s="369">
         <f>SUM(I11:I13)+SUM(I28:I30)</f>
         <v>6103303.7770000007</v>
       </c>
-      <c r="E53" s="437"/>
+      <c r="E53" s="435"/>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
     </row>
     <row r="54" spans="2:9" ht="14" x14ac:dyDescent="0.3">
       <c r="B54" s="83" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C54" s="6"/>
-      <c r="D54" s="436">
+      <c r="D54" s="434">
         <v>0</v>
       </c>
-      <c r="E54" s="388"/>
+      <c r="E54" s="359"/>
       <c r="F54" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G54" s="6"/>
     </row>
     <row r="55" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="83" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C55" s="6"/>
-      <c r="D55" s="436">
+      <c r="D55" s="434">
         <v>0</v>
       </c>
-      <c r="E55" s="388"/>
+      <c r="E55" s="359"/>
       <c r="F55" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G55" s="5"/>
     </row>
@@ -10603,17 +10679,17 @@
     </row>
     <row r="57" spans="2:9" ht="14" x14ac:dyDescent="0.3">
       <c r="B57" s="100" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C57" s="5"/>
-      <c r="D57" s="438"/>
-      <c r="E57" s="438"/>
+      <c r="D57" s="436"/>
+      <c r="E57" s="436"/>
       <c r="F57" s="19"/>
       <c r="G57" s="19"/>
     </row>
     <row r="58" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="57" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C58" s="274">
         <f>C14+C15+(C19*G19)+(C20*G20)+C29+C30+(C33*G33)+(C34*G34)+(C35*G35)</f>
@@ -10631,7 +10707,7 @@
     </row>
     <row r="59" spans="2:9" ht="14" x14ac:dyDescent="0.3">
       <c r="B59" s="57" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C59" s="274">
         <f>C11+C12+C28</f>
@@ -10650,14 +10726,14 @@
     </row>
     <row r="60" spans="2:9" ht="14" x14ac:dyDescent="0.3">
       <c r="B60" s="57" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C60" s="6"/>
-      <c r="D60" s="433">
+      <c r="D60" s="432">
         <f>((Dashboard!I6*Data!C4)+D52+E50-C58-C59)</f>
         <v>-11515263.40732</v>
       </c>
-      <c r="E60" s="434"/>
+      <c r="E60" s="433"/>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
     </row>
@@ -10666,17 +10742,15 @@
       <c r="E61" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="6">
     <mergeCell ref="D60:E60"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B9:D9"/>
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="D55:E55"/>
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="D53:E53"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation allowBlank="1" sqref="D49" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F33:F35 F19:F20" xr:uid="{DBDA56F9-BDA2-428A-9035-F60711F90E5E}">
       <formula1>"Y,N"</formula1>
@@ -10722,7 +10796,7 @@
     <row r="2" spans="1:11" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="123" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -10743,13 +10817,13 @@
         <v>44561</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E3" s="30">
         <v>1</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G3" s="30" t="str">
         <f>IF(G12="","","2")</f>
@@ -10760,12 +10834,12 @@
         <v/>
       </c>
       <c r="J3" s="97" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="17" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C4" s="285">
         <v>4053111</v>
@@ -10784,7 +10858,7 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C5" s="285">
         <v>1291010</v>
@@ -10803,7 +10877,7 @@
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="356" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C6" s="285">
         <f>C4+C5</f>
@@ -10829,7 +10903,7 @@
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C7" s="285">
         <v>4584914</v>
@@ -10848,7 +10922,7 @@
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C8" s="285">
         <v>3786145</v>
@@ -10867,7 +10941,7 @@
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="356" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C9" s="285">
         <f>C7+C8</f>
@@ -10893,7 +10967,7 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="356" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C10" s="285">
         <v>1611584</v>
@@ -10918,7 +10992,7 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C11" s="229">
         <f>C6+C9+C10</f>
@@ -10941,7 +11015,7 @@
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C12" s="236"/>
       <c r="D12" s="345"/>
@@ -10958,7 +11032,7 @@
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C13" s="230">
         <f>Data!C9</f>
@@ -10981,7 +11055,7 @@
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" s="235">
         <f>(C11-C13)/C11</f>
@@ -11000,7 +11074,7 @@
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C15" s="29">
         <f>C11-C13</f>
@@ -11022,7 +11096,7 @@
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="240">
         <f>C17/C11</f>
@@ -11041,7 +11115,7 @@
     </row>
     <row r="17" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C17" s="232">
         <v>2003343</v>
@@ -11062,7 +11136,7 @@
     </row>
     <row r="18" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="18">
         <f>C20/C11</f>
@@ -11085,7 +11159,7 @@
     </row>
     <row r="19" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C19" s="237"/>
       <c r="D19" s="348"/>
@@ -11105,7 +11179,7 @@
     </row>
     <row r="20" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="171" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C20" s="295">
         <f>C15-C17</f>
@@ -12038,8 +12112,8 @@
   </sheetPr>
   <dimension ref="A1:J926"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12060,7 +12134,7 @@
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="123" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -12091,15 +12165,15 @@
         <v/>
       </c>
       <c r="G3" s="30" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I3" s="97" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="231">
         <f>Operation!C20</f>
@@ -12124,7 +12198,7 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="17" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C5" s="338"/>
       <c r="D5" s="339">
@@ -12146,7 +12220,7 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C6" s="238">
         <v>0.16500000000000001</v>
@@ -12170,7 +12244,7 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" s="239">
         <f>IF(C4&lt;=0,C4,C4*(1-C6))</f>
@@ -12195,7 +12269,7 @@
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="90">
         <f>C10/C7</f>
@@ -12213,7 +12287,7 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C9" s="342"/>
       <c r="D9" s="340">
@@ -12228,7 +12302,7 @@
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="109" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C10" s="244">
         <v>2000000</v>
@@ -12252,7 +12326,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B11" s="17" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C11" s="243">
         <f>C7-C10</f>
@@ -12280,7 +12354,7 @@
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="260" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C12" s="297">
         <f>C11*Data!C$4/Dashboard!I5</f>
@@ -12308,7 +12382,7 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="307" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C13" s="299">
         <f>Data!C40/C12</f>
@@ -12327,7 +12401,7 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C14" s="310">
         <v>0</v>
@@ -12353,7 +12427,7 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C15" s="241"/>
       <c r="D15" s="286">
@@ -12378,7 +12452,7 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="111" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C16" s="146"/>
       <c r="D16" s="287">
@@ -12403,7 +12477,7 @@
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C17" s="311">
         <f>C14</f>
@@ -12435,19 +12509,19 @@
     </row>
     <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="27" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C19" s="246" t="str">
         <f>B3</f>
         <v>(Numbers in 1000HKD)</v>
       </c>
       <c r="E19" s="97" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="83" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C20" s="112">
         <f>'Asset Model'!E59</f>
@@ -12458,7 +12532,7 @@
         <v>11.676602903912285</v>
       </c>
       <c r="E20" s="113" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G20" s="174">
         <f>C20+C21+C22+C23</f>
@@ -12467,7 +12541,7 @@
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="83" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C21" s="112">
         <f>'Asset Model'!E58</f>
@@ -12478,7 +12552,7 @@
         <v>8.482979382201604</v>
       </c>
       <c r="E21" s="113" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G21" s="249">
         <f>G20*Data!C$4/Dashboard!I5</f>
@@ -12487,7 +12561,7 @@
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="83" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C22" s="112">
         <f>-'Asset Model'!D52</f>
@@ -12497,20 +12571,20 @@
         <f>C22/(Dashboard!I5/Data!C4)</f>
         <v>-4.2053758183007348</v>
       </c>
-      <c r="E22" s="441" t="str">
+      <c r="E22" s="439" t="str">
         <f>IF(F23+G23=G21,"⇒","Error!")</f>
         <v>⇒</v>
       </c>
       <c r="F22" s="185" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G22" s="116" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="113" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C23" s="112">
         <f>-'Asset Model'!E50</f>
@@ -12520,7 +12594,7 @@
         <f>C23/(Dashboard!I5/Data!C4)</f>
         <v>-0.57273456083900676</v>
       </c>
-      <c r="E23" s="441"/>
+      <c r="E23" s="439"/>
       <c r="F23" s="191">
         <f>D20</f>
         <v>11.676602903912285</v>
@@ -12536,17 +12610,17 @@
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="27" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C25" s="246" t="str">
         <f>B3</f>
         <v>(Numbers in 1000HKD)</v>
       </c>
       <c r="E25" s="114"/>
-      <c r="F25" s="440" t="s">
-        <v>311</v>
-      </c>
-      <c r="G25" s="440"/>
+      <c r="F25" s="438" t="s">
+        <v>309</v>
+      </c>
+      <c r="G25" s="438"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="164" t="str">
@@ -12554,22 +12628,22 @@
         <v>Exit after Year 1</v>
       </c>
       <c r="C26" s="164" t="s">
+        <v>305</v>
+      </c>
+      <c r="D26" s="257" t="s">
+        <v>295</v>
+      </c>
+      <c r="E26" s="164" t="s">
+        <v>306</v>
+      </c>
+      <c r="F26" s="353" t="s">
+        <v>308</v>
+      </c>
+      <c r="G26" s="353" t="s">
         <v>307</v>
       </c>
-      <c r="D26" s="257" t="s">
-        <v>297</v>
-      </c>
-      <c r="E26" s="164" t="s">
-        <v>308</v>
-      </c>
-      <c r="F26" s="353" t="s">
-        <v>310</v>
-      </c>
-      <c r="G26" s="353" t="s">
-        <v>309</v>
-      </c>
       <c r="I26" s="115" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -12590,7 +12664,7 @@
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="185" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C28" s="14">
         <f>1/D28</f>
@@ -12604,7 +12678,7 @@
         <f t="dataTable" ref="E28:E30" dt2D="0" dtr="0" r1="D27" ca="1"/>
         <v>3.8028951053470363</v>
       </c>
-      <c r="F28" s="442">
+      <c r="F28" s="440">
         <f ca="1">SUM(C17:F17)</f>
         <v>0.79594857520550355</v>
       </c>
@@ -12616,7 +12690,7 @@
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="185" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C29" s="14">
         <f t="shared" ref="C29" si="0">1/D29</f>
@@ -12629,7 +12703,7 @@
       <c r="E29" s="265">
         <v>4.9437636369511475</v>
       </c>
-      <c r="F29" s="443"/>
+      <c r="F29" s="441"/>
       <c r="G29" s="265">
         <f ca="1">$F$28+E29+$G$21</f>
         <v>21.121184119130799</v>
@@ -12638,7 +12712,7 @@
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="189" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C30" s="258">
         <f>1/D30</f>
@@ -12651,7 +12725,7 @@
       <c r="E30" s="267">
         <v>5.4381400006462632</v>
       </c>
-      <c r="F30" s="444"/>
+      <c r="F30" s="442"/>
       <c r="G30" s="267">
         <f ca="1">$F$28+E30+$G$21</f>
         <v>21.615560482825913</v>
@@ -12668,7 +12742,7 @@
     <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C32" s="331" t="str">
         <f>"(Numbers in "&amp;Dashboard!J4&amp;" per share)"</f>
@@ -12684,7 +12758,7 @@
     <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="96" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C33" s="333">
         <f ca="1">MIN('Asset Model'!D7,G28)+(ABS('Asset Model'!D7-G28)*'Qualitative Analysis'!E80)*Exchange_Rate</f>
@@ -12713,22 +12787,22 @@
       <c r="I34" s="119"/>
     </row>
     <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="358" t="s">
-        <v>191</v>
-      </c>
-      <c r="D35" s="439"/>
+      <c r="C35" s="403" t="s">
+        <v>189</v>
+      </c>
+      <c r="D35" s="437"/>
       <c r="E35" s="32" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F35" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G35" s="32"/>
       <c r="H35" s="6"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="337" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C36" s="334">
         <f ca="1">MIN(C33,E33)+(ABS(C33-E33)*'Qualitative Analysis'!E80)</f>
@@ -12752,7 +12826,7 @@
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="336" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C37" s="335">
         <f ca="1">(G14/(1+G37)^B27+F28+G21)*Exchange_Rate</f>
@@ -13709,7 +13783,7 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="11" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C2" s="126"/>
       <c r="D2" s="12"/>
@@ -13717,7 +13791,7 @@
     </row>
     <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="B3" s="127" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C3" s="128"/>
       <c r="D3" s="6"/>
@@ -13725,7 +13799,7 @@
     </row>
     <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C4" s="128"/>
       <c r="D4" s="125">
@@ -13733,12 +13807,12 @@
         <v>1</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C5" s="128"/>
       <c r="D5" s="125">
@@ -13746,12 +13820,12 @@
         <v>0</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C6" s="128"/>
       <c r="D6" s="125">
@@ -13759,12 +13833,12 @@
         <v>0</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="B7" s="129" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C7" s="128"/>
       <c r="D7" s="125">
@@ -13783,7 +13857,7 @@
     </row>
     <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="B9" s="131" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C9" s="57"/>
       <c r="D9" s="40"/>
@@ -13791,19 +13865,19 @@
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D10" s="132">
         <f>IF(E10="Strongly disagree",0,IF(E10="disagree",1,IF(E10="unclear",2,IF(E10="agree",3,4))))</f>
         <v>3</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C11" s="57"/>
       <c r="D11" s="132">
@@ -13817,7 +13891,7 @@
     </row>
     <row r="12" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D12" s="132">
         <f>IF(E12="Strongly disagree",0,IF(E12="disagree",1,IF(E12="unclear",2,IF(E12="agree",3,4))))</f>
@@ -13830,7 +13904,7 @@
     </row>
     <row r="13" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="B13" s="129" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D13" s="132">
         <f>AVERAGE(D10:D12)</f>
@@ -13849,17 +13923,17 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="B16" s="211" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="118">
@@ -13872,7 +13946,7 @@
     </row>
     <row r="17" spans="1:6" ht="14" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="132" t="str">
@@ -13880,37 +13954,37 @@
         <v>-</v>
       </c>
       <c r="E17" s="33" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="14" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D18" s="132" t="str">
         <f t="shared" ref="D18:D19" si="1">IF(LEFT(E18,3)="(+)","+","-")</f>
         <v>-</v>
       </c>
       <c r="E18" s="187" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D19" s="132" t="str">
         <f t="shared" si="1"/>
         <v>+</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="14" x14ac:dyDescent="0.3">
       <c r="B20" s="129" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D20" s="132" t="str">
         <f>D17&amp;D18&amp;D19</f>
@@ -13923,7 +13997,7 @@
     </row>
     <row r="21" spans="1:6" ht="14" x14ac:dyDescent="0.3">
       <c r="B21" s="129" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D21" s="118">
         <f>1/E21</f>
@@ -13941,7 +14015,7 @@
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
@@ -13949,14 +14023,14 @@
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="131" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C24" s="124"/>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="57" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D25" s="132">
         <f>IF(E25="Strongly disagree",0,IF(E25="disagree",1,IF(E25="unclear",2,IF(E25="agree",3,4))))</f>
@@ -13970,66 +14044,66 @@
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="57" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D26" s="132">
         <f>IF(E26="Strongly disagree",0,IF(E26="disagree",1,IF(E26="unclear",2,IF(E26="agree",3,4))))</f>
         <v>2</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="57" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D27" s="132">
         <f>IF(E27="Strongly disagree",0,IF(E27="disagree",1,IF(E27="unclear",2,IF(E27="agree",3,4))))</f>
         <v>2</v>
       </c>
       <c r="E27" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F27" s="6"/>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="57" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D28" s="132">
         <f>IF(E28="Strongly disagree",0,IF(E28="disagree",1,IF(E28="unclear",2,IF(E28="agree",3,4))))</f>
         <v>2</v>
       </c>
       <c r="E28" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="57" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D29" s="132">
         <f>IF(E29="Strongly disagree",0,IF(E29="disagree",1,IF(E29="unclear",2,IF(E29="agree",3,4))))</f>
         <v>4</v>
       </c>
       <c r="E29" s="33" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="131" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D30" s="40"/>
       <c r="E30" s="24"/>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="57" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D31" s="132">
         <f>IF(E31="Strongly disagree",0,IF(E31="disagree",1,IF(E31="unclear",2,IF(E31="agree",3,4))))</f>
@@ -14045,138 +14119,138 @@
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="57" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D32" s="132">
         <f t="shared" ref="D32:D35" si="2">IF(E32="Strongly disagree",0,IF(E32="disagree",1,IF(E32="unclear",2,IF(E32="agree",3,4))))</f>
         <v>1</v>
       </c>
       <c r="E32" s="33" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F32" s="6"/>
     </row>
     <row r="33" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="57" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D33" s="132">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F33" s="6"/>
     </row>
     <row r="34" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="57" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D34" s="132">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E34" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F34" s="6"/>
     </row>
     <row r="35" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="57" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D35" s="132">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E35" s="33" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F35" s="6"/>
     </row>
     <row r="36" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="131" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D36" s="40"/>
       <c r="E36" s="24"/>
     </row>
     <row r="37" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="57" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D37" s="132">
         <f t="shared" ref="D37:D41" si="3">IF(E37="Strongly disagree",0,IF(E37="disagree",1,IF(E37="unclear",2,IF(E37="agree",3,4))))</f>
         <v>4</v>
       </c>
       <c r="E37" s="33" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F37" s="6"/>
     </row>
     <row r="38" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="57" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D38" s="132">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E38" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F38" s="6"/>
     </row>
     <row r="39" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="57" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D39" s="132">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E39" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F39" s="6"/>
     </row>
     <row r="40" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="57" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D40" s="132">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="E40" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F40" s="6"/>
     </row>
     <row r="41" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="57" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D41" s="132">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E41" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F41" s="6"/>
     </row>
     <row r="42" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="131" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D42" s="40"/>
       <c r="E42" s="24"/>
     </row>
     <row r="43" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D43" s="135">
         <f>SUM(D44:D49)/(6*4)</f>
@@ -14190,84 +14264,84 @@
     </row>
     <row r="44" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="57" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D44" s="132">
         <f t="shared" ref="D44:D49" si="4">IF(E44="Strongly disagree",0,IF(E44="disagree",1,IF(E44="unclear",2,IF(E44="agree",3,4))))</f>
         <v>2</v>
       </c>
       <c r="E44" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F44" s="6"/>
     </row>
     <row r="45" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="57" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D45" s="132">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="E45" s="33" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F45" s="6"/>
     </row>
     <row r="46" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="57" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D46" s="132">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="E46" s="33" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F46" s="6"/>
     </row>
     <row r="47" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="57" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D47" s="132">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E47" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F47" s="6"/>
     </row>
     <row r="48" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="57" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D48" s="132">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="E48" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F48" s="6"/>
     </row>
     <row r="49" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="57" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D49" s="132">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="E49" s="33" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="50" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D50" s="135">
         <f>SUM(D51:D56)/(6*4)</f>
@@ -14281,84 +14355,84 @@
     </row>
     <row r="51" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="57" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D51" s="132">
         <f t="shared" ref="D51:D56" si="5">IF(E51="Strongly disagree",0,IF(E51="disagree",1,IF(E51="unclear",2,IF(E51="agree",3,4))))</f>
         <v>0</v>
       </c>
       <c r="E51" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F51" s="6"/>
     </row>
     <row r="52" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="57" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D52" s="132">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E52" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F52" s="6"/>
     </row>
     <row r="53" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="57" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D53" s="132">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E53" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F53" s="6"/>
     </row>
     <row r="54" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="57" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D54" s="132">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E54" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F54" s="6"/>
     </row>
     <row r="55" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="57" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D55" s="132">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E55" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F55" s="6"/>
     </row>
     <row r="56" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="57" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D56" s="132">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E56" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="57" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D57" s="135">
         <f>SUM(D58:D63)/(6*4)</f>
@@ -14372,85 +14446,85 @@
     </row>
     <row r="58" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="57" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D58" s="132">
         <f t="shared" ref="D58:D63" si="6">IF(E58="Strongly disagree",0,IF(E58="disagree",1,IF(E58="unclear",2,IF(E58="agree",3,4))))</f>
         <v>1</v>
       </c>
       <c r="E58" s="33" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F58" s="6"/>
     </row>
     <row r="59" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="57" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D59" s="132">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E59" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F59" s="6"/>
     </row>
     <row r="60" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="57" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D60" s="132">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="E60" s="33" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F60" s="6"/>
     </row>
     <row r="61" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="57" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D61" s="132">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E61" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F61" s="6"/>
     </row>
     <row r="62" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="57" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D62" s="132">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="E62" s="33" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F62" s="6"/>
     </row>
     <row r="63" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="57" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D63" s="132">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E63" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F63" s="6"/>
     </row>
     <row r="64" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D64" s="135">
         <f>SUM(D65:D70)/(6*4)</f>
@@ -14464,64 +14538,64 @@
     </row>
     <row r="65" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="57" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D65" s="132">
         <f t="shared" ref="D65:D68" si="7">IF(E65="Strongly disagree",0,IF(E65="disagree",1,IF(E65="unclear",2,IF(E65="agree",3,4))))</f>
         <v>0</v>
       </c>
       <c r="E65" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="66" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="57" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D66" s="132">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E66" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F66" s="6"/>
     </row>
     <row r="67" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="57" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D67" s="132">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E67" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="57" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D68" s="132">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="E68" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="69" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="57" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D69" s="132">
         <f>IF(E69="Strongly disagree",0,IF(E69="disagree",1,IF(E69="unclear",2,IF(E69="agree",3,4))))</f>
         <v>2</v>
       </c>
       <c r="E69" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F69" s="57"/>
       <c r="G69" s="57"/>
@@ -14529,14 +14603,14 @@
     </row>
     <row r="70" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="57" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D70" s="136">
         <f t="array" ref="D70">(1-INDEX(B84:E93,MATCH(E70,B84:B93,0),4))*4</f>
         <v>1.9455782312925169</v>
       </c>
       <c r="E70" s="33" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F70" s="57"/>
       <c r="G70" s="57"/>
@@ -14544,7 +14618,7 @@
     </row>
     <row r="71" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D71" s="137">
         <f>SUM(D72:D77)/(6*4)</f>
@@ -14560,14 +14634,14 @@
     </row>
     <row r="72" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="57" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D72" s="132">
         <f t="shared" ref="D72:D76" si="8">IF(E72="Strongly disagree",0,IF(E72="disagree",1,IF(E72="unclear",2,IF(E72="agree",3,4))))</f>
         <v>3</v>
       </c>
       <c r="E72" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F72" s="57"/>
       <c r="G72" s="57"/>
@@ -14575,14 +14649,14 @@
     </row>
     <row r="73" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="57" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D73" s="132">
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="E73" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F73" s="57"/>
       <c r="G73" s="57"/>
@@ -14590,14 +14664,14 @@
     </row>
     <row r="74" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="57" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D74" s="132">
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="E74" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F74" s="57"/>
       <c r="G74" s="57"/>
@@ -14605,14 +14679,14 @@
     </row>
     <row r="75" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="57" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D75" s="132">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="E75" s="33" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F75" s="57"/>
       <c r="G75" s="57"/>
@@ -14620,14 +14694,14 @@
     </row>
     <row r="76" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="57" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D76" s="132">
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="E76" s="33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F76" s="57"/>
       <c r="G76" s="57"/>
@@ -14635,14 +14709,14 @@
     </row>
     <row r="77" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="57" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D77" s="132">
         <f>IF(E77="Strongly disagree",0,IF(E77="disagree",1,IF(E77="non-perishable",2,IF(E77="agree",3,4))))</f>
         <v>0</v>
       </c>
       <c r="E77" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F77" s="57"/>
       <c r="G77" s="57"/>
@@ -14650,7 +14724,7 @@
     </row>
     <row r="78" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" s="185" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D78" s="163">
         <f>1-AVERAGE(D43,D50,D57,D64,D71)</f>
@@ -14669,7 +14743,7 @@
     </row>
     <row r="80" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="129" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D80" s="125">
         <f>E80*4</f>
@@ -14682,7 +14756,7 @@
     </row>
     <row r="82" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="58" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
@@ -14690,7 +14764,7 @@
     </row>
     <row r="83" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="138" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C83" s="139"/>
       <c r="D83" s="139"/>
@@ -14698,7 +14772,7 @@
     </row>
     <row r="84" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="141" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C84" s="139"/>
       <c r="D84" s="139">
@@ -14715,7 +14789,7 @@
         <v>Information Technology Like, 6.6y</v>
       </c>
       <c r="C85" s="139" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D85" s="139">
         <v>6.6</v>
@@ -14731,7 +14805,7 @@
         <v>Healthcare, 11.4y</v>
       </c>
       <c r="C86" s="139" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D86" s="139">
         <v>11.4</v>
@@ -14747,7 +14821,7 @@
         <v>Consumer Discretionary, 12.4y</v>
       </c>
       <c r="C87" s="139" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D87" s="139">
         <v>12.4</v>
@@ -14763,7 +14837,7 @@
         <v>Consumer Staples, 15.1y</v>
       </c>
       <c r="C88" s="139" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D88" s="139">
         <v>15.1</v>
@@ -14779,7 +14853,7 @@
         <v>Industrials, 15.4y</v>
       </c>
       <c r="C89" s="139" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D89" s="139">
         <v>15.4</v>
@@ -14795,7 +14869,7 @@
         <v>Telecommunication Services, 16.1y</v>
       </c>
       <c r="C90" s="139" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D90" s="139">
         <v>16.100000000000001</v>
@@ -14811,7 +14885,7 @@
         <v>Energy, 17.6y</v>
       </c>
       <c r="C91" s="139" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D91" s="139">
         <v>17.600000000000001</v>
@@ -14827,7 +14901,7 @@
         <v>Materials, 18.6y</v>
       </c>
       <c r="C92" s="139" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D92" s="139">
         <v>18.600000000000001</v>
@@ -14843,7 +14917,7 @@
         <v>Utilities, 29.4y</v>
       </c>
       <c r="C93" s="144" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D93" s="144">
         <v>29.4</v>

</xml_diff>